<commit_message>
relocalise make_planif_file in configuration AND add Tutor list and roomtype list validators!
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_planif_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_planif_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -66,6 +66,9 @@
     <t xml:space="preserve">Si aucun prof n’est indiqué, c’est un cours supposé en autonomie</t>
   </si>
   <si>
+    <t xml:space="preserve">Voici la liste des profs possibles :</t>
+  </si>
+  <si>
     <t xml:space="preserve">Type de salle </t>
   </si>
   <si>
@@ -73,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve">Si les cours doivent avoir des types de salle différents, faites plusieurs lignes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voici la liste des types de salle possibles :</t>
   </si>
   <si>
     <t xml:space="preserve">Mode de remplissage des cours</t>
@@ -139,10 +145,7 @@
     <t xml:space="preserve">Après le premier cours de type « type » de la semaine</t>
   </si>
   <si>
-    <t xml:space="preserve">(Ex : ATD, ACM, ATP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB : pour que le ATD fonctionne, il faut que le TD soit au dessus dans le tableau !</t>
+    <t xml:space="preserve">(Ex : ATD, ACM, ATP) NB : pour que le ATD fonctionne, il faut que le TD soit au dessus dans le tableau ! </t>
   </si>
   <si>
     <r>
@@ -554,7 +557,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -687,7 +690,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -782,7 +789,7 @@
   </sheetPr>
   <dimension ref="A1:DG9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2418,16 +2425,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="2" style="0" width="11.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="2" style="0" width="6.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="136" style="0" width="11.34"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -2498,11 +2506,9 @@
       <c r="I5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="30" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31"/>
@@ -2513,114 +2519,115 @@
       <c r="I6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="29"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="29"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="28" t="s">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="30" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="30"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29"/>
-      <c r="B11" s="32" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="29"/>
+      <c r="B16" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
-      <c r="B13" s="32" t="s">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29"/>
-      <c r="B14" s="32" t="s">
+      <c r="B17" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="30"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="s">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="29"/>
+      <c r="B18" s="32" t="s">
         <v>25</v>
-      </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="30" t="s">
-        <v>27</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -2631,11 +2638,9 @@
       <c r="I18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="30" t="s">
-        <v>29</v>
+      <c r="A19" s="29"/>
+      <c r="B19" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -2645,38 +2650,25 @@
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-    </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
+      <c r="A21" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="29"/>
+      <c r="A22" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="B22" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
@@ -2686,12 +2678,12 @@
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
@@ -2702,8 +2694,74 @@
       <c r="I23" s="31"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="33" t="s">
+      <c r="A24" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="29"/>
+      <c r="B25" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+      <c r="I25" s="31"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="29"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="30" t="s">
         <v>36</v>
+      </c>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="34" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2743,10 +2801,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="34" t="s">
         <v>38</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>39</v>
       </c>
       <c r="C1" s="3" t="n">
         <v>35</v>
@@ -3078,56 +3136,56 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="36"/>
-      <c r="AC3" s="36"/>
-      <c r="AD3" s="36"/>
-      <c r="AE3" s="36"/>
-      <c r="AF3" s="36"/>
-      <c r="AG3" s="36"/>
-      <c r="AH3" s="36"/>
-      <c r="AI3" s="36"/>
-      <c r="AJ3" s="36"/>
-      <c r="AK3" s="36"/>
-      <c r="AL3" s="36"/>
-      <c r="AM3" s="36"/>
-      <c r="AN3" s="36"/>
-      <c r="AO3" s="36"/>
-      <c r="AP3" s="36"/>
-      <c r="AQ3" s="36"/>
-      <c r="AR3" s="36"/>
-      <c r="AS3" s="36"/>
-      <c r="AT3" s="36"/>
-      <c r="AU3" s="36"/>
-      <c r="AV3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="37"/>
+      <c r="AP3" s="37"/>
+      <c r="AQ3" s="37"/>
+      <c r="AR3" s="37"/>
+      <c r="AS3" s="37"/>
+      <c r="AT3" s="37"/>
+      <c r="AU3" s="37"/>
+      <c r="AV3" s="37"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
visio remarks in planif_file
</commit_message>
<xml_diff>
--- a/FlOpEDT/media/configuration/empty_planif_file.xlsx
+++ b/FlOpEDT/media/configuration/empty_planif_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t xml:space="preserve">(Ex : A3TD, A2CM, A1TP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seulement pour le Visio-Mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le cours ne peut pas se faire en distanciel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le cours doit se faire en distanciel</t>
   </si>
   <si>
     <t xml:space="preserve">Enseignant</t>
@@ -2539,10 +2554,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2876,6 +2891,27 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="34" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2915,10 +2951,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C1" s="3" t="n">
         <v>35</v>
@@ -3319,15 +3355,15 @@
   </sheetPr>
   <dimension ref="A1:O99"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="0" width="16.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="0" width="16.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -3339,7 +3375,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
@@ -3377,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -3416,7 +3452,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
@@ -3455,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
@@ -3494,7 +3530,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C9" s="44"/>
       <c r="D9" s="44"/>
@@ -3533,7 +3569,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C11" s="44"/>
       <c r="D11" s="44"/>
@@ -3572,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="B13" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C13" s="44"/>
       <c r="D13" s="44"/>
@@ -3611,7 +3647,7 @@
         <v>0</v>
       </c>
       <c r="B15" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C15" s="44"/>
       <c r="D15" s="44"/>
@@ -3650,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="44"/>
@@ -3689,7 +3725,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="44"/>
@@ -3728,7 +3764,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C21" s="44"/>
       <c r="D21" s="44"/>
@@ -3767,7 +3803,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="44"/>
@@ -3806,7 +3842,7 @@
         <v>0</v>
       </c>
       <c r="B25" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
@@ -3845,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="44"/>
@@ -3884,7 +3920,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C29" s="44"/>
       <c r="D29" s="44"/>
@@ -3923,7 +3959,7 @@
         <v>0</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="44"/>
@@ -3962,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="44"/>
@@ -4001,7 +4037,7 @@
         <v>0</v>
       </c>
       <c r="B35" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C35" s="44"/>
       <c r="D35" s="44"/>
@@ -4040,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C37" s="44"/>
       <c r="D37" s="44"/>
@@ -4079,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C39" s="44"/>
       <c r="D39" s="44"/>
@@ -4118,7 +4154,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C41" s="44"/>
       <c r="D41" s="44"/>
@@ -4157,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C43" s="44"/>
       <c r="D43" s="44"/>
@@ -4196,7 +4232,7 @@
         <v>0</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C45" s="44"/>
       <c r="D45" s="44"/>
@@ -4235,7 +4271,7 @@
         <v>0</v>
       </c>
       <c r="B47" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C47" s="44"/>
       <c r="D47" s="44"/>
@@ -4274,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="44"/>
@@ -4313,7 +4349,7 @@
         <v>0</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C51" s="44"/>
       <c r="D51" s="44"/>
@@ -4352,7 +4388,7 @@
         <v>0</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C53" s="44"/>
       <c r="D53" s="44"/>
@@ -4391,7 +4427,7 @@
         <v>0</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C55" s="44"/>
       <c r="D55" s="44"/>
@@ -4430,7 +4466,7 @@
         <v>0</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C57" s="44"/>
       <c r="D57" s="44"/>
@@ -4469,7 +4505,7 @@
         <v>0</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C59" s="44"/>
       <c r="D59" s="44"/>
@@ -4508,7 +4544,7 @@
         <v>0</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C61" s="44"/>
       <c r="D61" s="44"/>
@@ -4547,7 +4583,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C63" s="44"/>
       <c r="D63" s="44"/>
@@ -4586,7 +4622,7 @@
         <v>0</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C65" s="44"/>
       <c r="D65" s="44"/>
@@ -4625,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C67" s="44"/>
       <c r="D67" s="44"/>
@@ -4664,7 +4700,7 @@
         <v>0</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C69" s="44"/>
       <c r="D69" s="44"/>
@@ -4703,7 +4739,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C71" s="44"/>
       <c r="D71" s="44"/>
@@ -4742,7 +4778,7 @@
         <v>0</v>
       </c>
       <c r="B73" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C73" s="44"/>
       <c r="D73" s="44"/>
@@ -4781,7 +4817,7 @@
         <v>0</v>
       </c>
       <c r="B75" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C75" s="44"/>
       <c r="D75" s="44"/>
@@ -4820,7 +4856,7 @@
         <v>0</v>
       </c>
       <c r="B77" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C77" s="44"/>
       <c r="D77" s="44"/>
@@ -4859,7 +4895,7 @@
         <v>0</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C79" s="44"/>
       <c r="D79" s="44"/>
@@ -4898,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C81" s="44"/>
       <c r="D81" s="44"/>
@@ -4937,7 +4973,7 @@
         <v>0</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C83" s="44"/>
       <c r="D83" s="44"/>
@@ -4976,7 +5012,7 @@
         <v>0</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C85" s="44"/>
       <c r="D85" s="44"/>
@@ -5015,7 +5051,7 @@
         <v>0</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C87" s="44"/>
       <c r="D87" s="44"/>
@@ -5054,7 +5090,7 @@
         <v>0</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C89" s="44"/>
       <c r="D89" s="44"/>
@@ -5093,7 +5129,7 @@
         <v>0</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C91" s="44"/>
       <c r="D91" s="44"/>
@@ -5132,7 +5168,7 @@
         <v>0</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C93" s="44"/>
       <c r="D93" s="44"/>
@@ -5171,7 +5207,7 @@
         <v>0</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C95" s="44"/>
       <c r="D95" s="44"/>
@@ -5210,7 +5246,7 @@
         <v>0</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C97" s="44"/>
       <c r="D97" s="44"/>
@@ -5249,7 +5285,7 @@
         <v>0</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C99" s="44"/>
       <c r="D99" s="44"/>

</xml_diff>